<commit_message>
CharacterSpawnData 데이터 가공 추가
기존 MonsterSpawnData 대신 CharacterSpawnData로 변경
</commit_message>
<xml_diff>
--- a/DataGenerator/XLSXS/CharacterSpawnData.xlsx
+++ b/DataGenerator/XLSXS/CharacterSpawnData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jehee\Documents\GitHub\DG_Project\DataGenerator\XLSXS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunja\Documents\DG_Project\DataGenerator\XLSXS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE451324-45BD-4F21-B288-78657E14E441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D887FA-34D8-44BE-A00B-81329CC475EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4515" yWindow="3690" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23865" yWindow="2670" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="시트8" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Index</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>위치는 20.22.32.33</t>
+  </si>
+  <si>
+    <t>SpawnID</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -489,7 +492,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -573,7 +578,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>1500100</v>
       </c>
@@ -631,7 +636,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>1500102</v>
       </c>
@@ -660,7 +665,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>1500103</v>
       </c>
@@ -718,7 +723,7 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>1500105</v>
       </c>
@@ -772,7 +777,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>1201</v>
       </c>
@@ -826,7 +831,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>1203</v>
       </c>

</xml_diff>